<commit_message>
Bitacora y coevaluacion completados
</commit_message>
<xml_diff>
--- a/EQUIPO 1-BITÁCORA 1P.xlsx
+++ b/EQUIPO 1-BITÁCORA 1P.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Desktop\UTCV\5to\Proyecto\Bitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B41CB7F-6502-4279-B909-2991F9668CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2943AB-8B77-4B8B-B49C-DE7F7E80FD19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATOS GENERALES" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="95">
   <si>
     <r>
       <rPr>
@@ -224,9 +224,6 @@
     <t>PARCIAL 2</t>
   </si>
   <si>
-    <t>Recopilación de datos</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
@@ -346,28 +343,10 @@
     <t>Desarollar la pagina web y una aplicacion movil de una barbería en Córdoba, Veracruz</t>
   </si>
   <si>
-    <t>Creacion de app android</t>
-  </si>
-  <si>
-    <t>Recopilacion de datos bajo estandares de proyecto pasados y las expectativas actuales.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creacion de Aplicacion </t>
-  </si>
-  <si>
-    <t>Apis</t>
-  </si>
-  <si>
-    <t>Pruebas</t>
-  </si>
-  <si>
     <t>Periodo y documentacion de pruebas</t>
   </si>
   <si>
     <t>Respaldo</t>
-  </si>
-  <si>
-    <t>Creacion y uso de apis</t>
   </si>
   <si>
     <t>20233l001139</t>
@@ -419,6 +398,48 @@
   </si>
   <si>
     <t>Integracion y cooperacion para desarrollar appMovil</t>
+  </si>
+  <si>
+    <t>Resolver problemas que surgieron al realizar los rubros de el checklist aportando ideas</t>
+  </si>
+  <si>
+    <t>Lograr el mayor avance posible hacia el apartado de AppMovil y Industria 4.0</t>
+  </si>
+  <si>
+    <t>Recopilación de Informacion</t>
+  </si>
+  <si>
+    <t>requerimientos del proyecto</t>
+  </si>
+  <si>
+    <t>Desarrollo de Aplicacion Movil</t>
+  </si>
+  <si>
+    <t>Recopilacion de informacion en base a los</t>
+  </si>
+  <si>
+    <t>Discusión y resolución de problemas</t>
+  </si>
+  <si>
+    <t>Análisis de los problemas encontrados en el checklist, propuesta de soluciones y toma de acuerdos para su implementación.</t>
+  </si>
+  <si>
+    <t>Se busco avanzar mas la parte de la appMovil en ionic y landing en angular, tambien se subio el avanze a un repositorio git por posibles fallas.</t>
+  </si>
+  <si>
+    <t>Compromiso de los participantes para involucrarse activamente en la resolución de problemas, estableciendo tareas y responsabilidades específicas.</t>
+  </si>
+  <si>
+    <t>Se investigó sobre el prototipo IoT y se inició la elaboración de su diagrama, identificando los elementos clave y su funcionamiento dentro del proyecto.</t>
+  </si>
+  <si>
+    <t>Cada integrante se comprometió a integrarse activamente para completar el diagrama del prototipo IoT y cumplir con los requisitos establecidos en el checklist.</t>
+  </si>
+  <si>
+    <t>Análisis y modelado del sistema IOT</t>
+  </si>
+  <si>
+    <t>Creacion y desarrollo para el avance de la app Movil</t>
   </si>
 </sst>
 </file>
@@ -873,7 +894,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1022,6 +1043,21 @@
     <xf numFmtId="44" fontId="13" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1250,6 +1286,471 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1018540</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B85FF9D3-DF68-4C8F-AAD3-B67E3A195361}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914400" y="6530340"/>
+          <a:ext cx="2580640" cy="1935480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1082040</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1493520</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>148792</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5EA09C5-6289-4347-A8BB-40B8580F21B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3558540" y="6522720"/>
+          <a:ext cx="3398520" cy="1909012"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1066800</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0C9EC78-C81F-4493-90E5-04063130E2D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1943100" y="8442960"/>
+          <a:ext cx="3710940" cy="1577340"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>157270</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84399B11-E9BE-494E-92FD-61A827F8E53D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1028700" y="6873240"/>
+          <a:ext cx="3253740" cy="2557570"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>190502</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1391325</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>122984</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85364571-F183-4D49-8714-50FB9347A107}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4434840" y="7086602"/>
+          <a:ext cx="2420025" cy="2111802"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>115204</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1226514</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F486EC25-6DC6-4031-9842-86447D08B491}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="937260" y="6615064"/>
+          <a:ext cx="2765754" cy="1553576"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>177652</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>67644</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1386840</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C94499D-81CB-4821-A2FA-275C066D37A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4284832" y="6567504"/>
+          <a:ext cx="2565548" cy="1441116"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1188720</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>100399</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D42085AE-02F8-4C30-8E65-CA7F1541BD87}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1112520" y="8534400"/>
+          <a:ext cx="2552700" cy="1433899"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1600200</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>53100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1203960</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>121561</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagen 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC39EF15-86C2-4630-98C3-54E426C59CFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4076700" y="8534160"/>
+          <a:ext cx="2590800" cy="1455301"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
 <richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rel r:id="rId1"/>
@@ -1464,8 +1965,8 @@
   </sheetPr>
   <dimension ref="B1:E999"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -1515,7 +2016,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>3</v>
@@ -1539,7 +2040,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="47"/>
       <c r="E10" s="48"/>
@@ -1569,16 +2070,16 @@
     </row>
     <row r="14" spans="2:5" ht="15.75" customHeight="1">
       <c r="B14" s="4" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="15.75" customHeight="1">
@@ -1625,30 +2126,30 @@
     </row>
     <row r="18" spans="2:5" ht="15.75" customHeight="1">
       <c r="B18" s="27" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="15.75" customHeight="1">
       <c r="B19" s="27" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="15.75" customHeight="1">
@@ -2721,7 +3222,7 @@
     <row r="6" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="7" spans="2:5" ht="30.75" customHeight="1">
       <c r="B7" s="74" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="47"/>
       <c r="D7" s="47"/>
@@ -2730,15 +3231,15 @@
     <row r="8" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="9" spans="2:5" ht="15.75" customHeight="1">
       <c r="B9" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" customHeight="1">
       <c r="B10" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="75">
         <v>45667</v>
@@ -2748,20 +3249,20 @@
     </row>
     <row r="11" spans="2:5" ht="15.75" customHeight="1">
       <c r="B11" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="76" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="47"/>
       <c r="E11" s="48"/>
     </row>
     <row r="12" spans="2:5" ht="50.25" customHeight="1">
       <c r="B12" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="47"/>
       <c r="E12" s="48"/>
@@ -2769,7 +3270,7 @@
     <row r="13" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="14" spans="2:5" ht="15.75" customHeight="1">
       <c r="B14" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="47"/>
       <c r="D14" s="47"/>
@@ -2813,7 +3314,7 @@
     </row>
     <row r="21" spans="2:5" ht="15.75" customHeight="1">
       <c r="B21" s="77" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="47"/>
       <c r="D21" s="47"/>
@@ -2821,7 +3322,7 @@
     </row>
     <row r="22" spans="2:5" ht="15.75" customHeight="1">
       <c r="B22" s="78" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" s="39"/>
       <c r="D22" s="39"/>
@@ -2859,7 +3360,7 @@
     </row>
     <row r="28" spans="2:5" ht="15.75" customHeight="1">
       <c r="B28" s="77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="47"/>
@@ -2981,7 +3482,7 @@
     </row>
     <row r="48" spans="2:5" ht="15.75" customHeight="1">
       <c r="B48" s="77" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" s="47"/>
       <c r="D48" s="47"/>
@@ -2989,7 +3490,7 @@
     </row>
     <row r="49" spans="2:5" ht="15.75" customHeight="1">
       <c r="B49" s="73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49" s="39"/>
       <c r="D49" s="39"/>
@@ -4045,7 +4546,7 @@
     <row r="6" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="7" spans="2:5" ht="30.75" customHeight="1">
       <c r="B7" s="74" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="47"/>
       <c r="D7" s="47"/>
@@ -4054,15 +4555,15 @@
     <row r="8" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="9" spans="2:5" ht="15.75" customHeight="1">
       <c r="B9" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" customHeight="1">
       <c r="B10" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="75">
         <v>45667</v>
@@ -4072,20 +4573,20 @@
     </row>
     <row r="11" spans="2:5" ht="15.75" customHeight="1">
       <c r="B11" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="76" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="47"/>
       <c r="E11" s="48"/>
     </row>
     <row r="12" spans="2:5" ht="50.25" customHeight="1">
       <c r="B12" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="47"/>
       <c r="E12" s="48"/>
@@ -4093,7 +4594,7 @@
     <row r="13" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="14" spans="2:5" ht="15.75" customHeight="1">
       <c r="B14" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="47"/>
       <c r="D14" s="47"/>
@@ -4137,7 +4638,7 @@
     </row>
     <row r="21" spans="2:5" ht="15.75" customHeight="1">
       <c r="B21" s="77" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="47"/>
       <c r="D21" s="47"/>
@@ -4145,7 +4646,7 @@
     </row>
     <row r="22" spans="2:5" ht="15.75" customHeight="1">
       <c r="B22" s="78" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" s="39"/>
       <c r="D22" s="39"/>
@@ -4183,7 +4684,7 @@
     </row>
     <row r="28" spans="2:5" ht="15.75" customHeight="1">
       <c r="B28" s="77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="47"/>
@@ -4305,7 +4806,7 @@
     </row>
     <row r="48" spans="2:5" ht="15.75" customHeight="1">
       <c r="B48" s="77" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" s="47"/>
       <c r="D48" s="47"/>
@@ -4313,7 +4814,7 @@
     </row>
     <row r="49" spans="2:5" ht="15.75" customHeight="1">
       <c r="B49" s="73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49" s="39"/>
       <c r="D49" s="39"/>
@@ -5369,7 +5870,7 @@
     <row r="6" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="7" spans="2:5" ht="30.75" customHeight="1">
       <c r="B7" s="74" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="47"/>
       <c r="D7" s="47"/>
@@ -5378,15 +5879,15 @@
     <row r="8" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="9" spans="2:5" ht="15.75" customHeight="1">
       <c r="B9" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" customHeight="1">
       <c r="B10" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="75">
         <v>45667</v>
@@ -5396,20 +5897,20 @@
     </row>
     <row r="11" spans="2:5" ht="15.75" customHeight="1">
       <c r="B11" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="76" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="47"/>
       <c r="E11" s="48"/>
     </row>
     <row r="12" spans="2:5" ht="50.25" customHeight="1">
       <c r="B12" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="47"/>
       <c r="E12" s="48"/>
@@ -5417,7 +5918,7 @@
     <row r="13" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="14" spans="2:5" ht="15.75" customHeight="1">
       <c r="B14" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="47"/>
       <c r="D14" s="47"/>
@@ -5461,7 +5962,7 @@
     </row>
     <row r="21" spans="2:5" ht="15.75" customHeight="1">
       <c r="B21" s="77" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="47"/>
       <c r="D21" s="47"/>
@@ -5469,7 +5970,7 @@
     </row>
     <row r="22" spans="2:5" ht="15.75" customHeight="1">
       <c r="B22" s="78" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" s="39"/>
       <c r="D22" s="39"/>
@@ -5507,7 +6008,7 @@
     </row>
     <row r="28" spans="2:5" ht="15.75" customHeight="1">
       <c r="B28" s="77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="47"/>
@@ -5629,7 +6130,7 @@
     </row>
     <row r="48" spans="2:5" ht="15.75" customHeight="1">
       <c r="B48" s="77" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" s="47"/>
       <c r="D48" s="47"/>
@@ -5637,7 +6138,7 @@
     </row>
     <row r="49" spans="2:5" ht="15.75" customHeight="1">
       <c r="B49" s="73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49" s="39"/>
       <c r="D49" s="39"/>
@@ -6693,7 +7194,7 @@
     <row r="6" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="7" spans="2:5" ht="30.75" customHeight="1">
       <c r="B7" s="74" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="47"/>
       <c r="D7" s="47"/>
@@ -6702,15 +7203,15 @@
     <row r="8" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="9" spans="2:5" ht="15.75" customHeight="1">
       <c r="B9" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" customHeight="1">
       <c r="B10" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="75">
         <v>45667</v>
@@ -6720,20 +7221,20 @@
     </row>
     <row r="11" spans="2:5" ht="15.75" customHeight="1">
       <c r="B11" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="76" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="47"/>
       <c r="E11" s="48"/>
     </row>
     <row r="12" spans="2:5" ht="50.25" customHeight="1">
       <c r="B12" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="47"/>
       <c r="E12" s="48"/>
@@ -6741,7 +7242,7 @@
     <row r="13" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="14" spans="2:5" ht="15.75" customHeight="1">
       <c r="B14" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="47"/>
       <c r="D14" s="47"/>
@@ -6785,7 +7286,7 @@
     </row>
     <row r="21" spans="2:5" ht="15.75" customHeight="1">
       <c r="B21" s="77" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="47"/>
       <c r="D21" s="47"/>
@@ -6793,7 +7294,7 @@
     </row>
     <row r="22" spans="2:5" ht="15.75" customHeight="1">
       <c r="B22" s="78" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" s="39"/>
       <c r="D22" s="39"/>
@@ -6831,7 +7332,7 @@
     </row>
     <row r="28" spans="2:5" ht="15.75" customHeight="1">
       <c r="B28" s="77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="47"/>
@@ -6953,7 +7454,7 @@
     </row>
     <row r="48" spans="2:5" ht="15.75" customHeight="1">
       <c r="B48" s="77" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" s="47"/>
       <c r="D48" s="47"/>
@@ -6961,7 +7462,7 @@
     </row>
     <row r="49" spans="2:5" ht="15.75" customHeight="1">
       <c r="B49" s="73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49" s="39"/>
       <c r="D49" s="39"/>
@@ -8017,7 +8518,7 @@
     <row r="6" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="7" spans="2:5" ht="30.75" customHeight="1">
       <c r="B7" s="74" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="47"/>
       <c r="D7" s="47"/>
@@ -8026,15 +8527,15 @@
     <row r="8" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="9" spans="2:5" ht="15.75" customHeight="1">
       <c r="B9" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" customHeight="1">
       <c r="B10" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="75">
         <v>45667</v>
@@ -8044,20 +8545,20 @@
     </row>
     <row r="11" spans="2:5" ht="15.75" customHeight="1">
       <c r="B11" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="76" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="47"/>
       <c r="E11" s="48"/>
     </row>
     <row r="12" spans="2:5" ht="50.25" customHeight="1">
       <c r="B12" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="47"/>
       <c r="E12" s="48"/>
@@ -8065,7 +8566,7 @@
     <row r="13" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="14" spans="2:5" ht="15.75" customHeight="1">
       <c r="B14" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="47"/>
       <c r="D14" s="47"/>
@@ -8109,7 +8610,7 @@
     </row>
     <row r="21" spans="2:5" ht="15.75" customHeight="1">
       <c r="B21" s="77" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="47"/>
       <c r="D21" s="47"/>
@@ -8117,7 +8618,7 @@
     </row>
     <row r="22" spans="2:5" ht="15.75" customHeight="1">
       <c r="B22" s="78" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" s="39"/>
       <c r="D22" s="39"/>
@@ -8155,7 +8656,7 @@
     </row>
     <row r="28" spans="2:5" ht="15.75" customHeight="1">
       <c r="B28" s="77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="47"/>
@@ -8277,7 +8778,7 @@
     </row>
     <row r="48" spans="2:5" ht="15.75" customHeight="1">
       <c r="B48" s="77" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" s="47"/>
       <c r="D48" s="47"/>
@@ -8285,7 +8786,7 @@
     </row>
     <row r="49" spans="2:5" ht="15.75" customHeight="1">
       <c r="B49" s="73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49" s="39"/>
       <c r="D49" s="39"/>
@@ -9341,7 +9842,7 @@
     <row r="6" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="7" spans="2:5" ht="30.75" customHeight="1">
       <c r="B7" s="74" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="47"/>
       <c r="D7" s="47"/>
@@ -9350,15 +9851,15 @@
     <row r="8" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="9" spans="2:5" ht="15.75" customHeight="1">
       <c r="B9" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" customHeight="1">
       <c r="B10" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="75">
         <v>45667</v>
@@ -9368,20 +9869,20 @@
     </row>
     <row r="11" spans="2:5" ht="15.75" customHeight="1">
       <c r="B11" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="76" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="47"/>
       <c r="E11" s="48"/>
     </row>
     <row r="12" spans="2:5" ht="50.25" customHeight="1">
       <c r="B12" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="79" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="80"/>
       <c r="E12" s="81"/>
@@ -9389,7 +9890,7 @@
     <row r="13" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="14" spans="2:5" ht="15.75" customHeight="1">
       <c r="B14" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="47"/>
       <c r="D14" s="47"/>
@@ -9433,7 +9934,7 @@
     </row>
     <row r="21" spans="2:5" ht="15.75" customHeight="1">
       <c r="B21" s="77" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="47"/>
       <c r="D21" s="47"/>
@@ -9441,7 +9942,7 @@
     </row>
     <row r="22" spans="2:5" ht="15.75" customHeight="1">
       <c r="B22" s="78" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" s="39"/>
       <c r="D22" s="39"/>
@@ -9479,7 +9980,7 @@
     </row>
     <row r="28" spans="2:5" ht="15.75" customHeight="1">
       <c r="B28" s="77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="47"/>
@@ -9601,7 +10102,7 @@
     </row>
     <row r="48" spans="2:5" ht="15.75" customHeight="1">
       <c r="B48" s="77" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" s="47"/>
       <c r="D48" s="47"/>
@@ -9609,7 +10110,7 @@
     </row>
     <row r="49" spans="2:5" ht="15.75" customHeight="1">
       <c r="B49" s="73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49" s="39"/>
       <c r="D49" s="39"/>
@@ -10624,8 +11125,8 @@
   </sheetPr>
   <dimension ref="B1:U1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -10850,18 +11351,18 @@
       <c r="B12" s="64">
         <v>1</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="C12" s="85" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="86"/>
+      <c r="E12" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+      <c r="H12" s="23"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -10878,14 +11379,16 @@
     </row>
     <row r="13" spans="2:21" ht="15.6" customHeight="1">
       <c r="B13" s="56"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="21"/>
+      <c r="C13" s="87"/>
+      <c r="D13" s="88"/>
+      <c r="E13" s="21" t="s">
+        <v>84</v>
+      </c>
       <c r="F13" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
+      <c r="H13" s="25"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
@@ -10905,14 +11408,14 @@
         <v>2</v>
       </c>
       <c r="C14" s="65" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" s="40"/>
       <c r="E14" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
@@ -10936,7 +11439,7 @@
       <c r="D15" s="46"/>
       <c r="E15" s="19"/>
       <c r="F15" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
@@ -10998,20 +11501,20 @@
     </row>
     <row r="18" spans="2:21" ht="13.5" customHeight="1">
       <c r="B18" s="64">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18" s="66" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="D18" s="40"/>
       <c r="E18" s="67" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
+      <c r="H18" s="22"/>
       <c r="I18" s="22"/>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
@@ -11032,15 +11535,15 @@
       <c r="D19" s="46"/>
       <c r="E19" s="46"/>
       <c r="F19" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
+      <c r="H19" s="24"/>
       <c r="I19" s="24"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="8"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="26"/>
       <c r="N19" s="8"/>
       <c r="O19" s="8"/>
       <c r="P19" s="8"/>
@@ -11052,140 +11555,140 @@
     </row>
     <row r="20" spans="2:21" ht="13.5" customHeight="1">
       <c r="B20" s="64">
-        <v>4</v>
-      </c>
-      <c r="C20" s="65" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="40"/>
+        <v>3</v>
+      </c>
+      <c r="C20" s="85" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="86"/>
       <c r="E20" s="67" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
+      <c r="I20" s="9"/>
       <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
-      <c r="T20" s="8"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="26"/>
+      <c r="Q20" s="26"/>
+      <c r="R20" s="26"/>
+      <c r="S20" s="26"/>
+      <c r="T20" s="26"/>
       <c r="U20" s="8"/>
     </row>
     <row r="21" spans="2:21" ht="15.75" customHeight="1">
       <c r="B21" s="56"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="46"/>
+      <c r="C21" s="87"/>
+      <c r="D21" s="88"/>
       <c r="E21" s="46"/>
       <c r="F21" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
+      <c r="I21" s="10"/>
       <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="24"/>
-      <c r="S21" s="8"/>
-      <c r="T21" s="8"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="26"/>
+      <c r="R21" s="26"/>
+      <c r="S21" s="26"/>
+      <c r="T21" s="26"/>
       <c r="U21" s="8"/>
     </row>
     <row r="22" spans="2:21" ht="13.5" customHeight="1">
       <c r="B22" s="64">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" s="72" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="40"/>
+        <v>93</v>
+      </c>
+      <c r="D22" s="82"/>
       <c r="E22" s="67" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="23"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="9"/>
       <c r="L22" s="23"/>
       <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="22"/>
-      <c r="S22" s="22"/>
-      <c r="T22" s="8"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="26"/>
+      <c r="R22" s="26"/>
+      <c r="S22" s="26"/>
+      <c r="T22" s="26"/>
       <c r="U22" s="8"/>
     </row>
     <row r="23" spans="2:21" ht="15.75" customHeight="1">
       <c r="B23" s="56"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="46"/>
+      <c r="C23" s="83"/>
+      <c r="D23" s="84"/>
       <c r="E23" s="46"/>
       <c r="F23" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
-      <c r="K23" s="25"/>
+      <c r="K23" s="10"/>
       <c r="L23" s="25"/>
       <c r="M23" s="26"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="24"/>
-      <c r="S23" s="24"/>
-      <c r="T23" s="8"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="26"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="26"/>
+      <c r="R23" s="26"/>
+      <c r="S23" s="26"/>
+      <c r="T23" s="26"/>
       <c r="U23" s="8"/>
     </row>
     <row r="24" spans="2:21" ht="13.5" customHeight="1">
       <c r="B24" s="64">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" s="69" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D24" s="40"/>
       <c r="E24" s="67" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
+      <c r="K24" s="9"/>
       <c r="L24" s="8"/>
       <c r="M24" s="26"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="22"/>
-      <c r="T24" s="22"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="26"/>
+      <c r="Q24" s="26"/>
+      <c r="R24" s="26"/>
+      <c r="S24" s="26"/>
+      <c r="T24" s="26"/>
       <c r="U24" s="8"/>
     </row>
     <row r="25" spans="2:21" ht="15.75" customHeight="1">
@@ -11194,33 +11697,33 @@
       <c r="D25" s="46"/>
       <c r="E25" s="46"/>
       <c r="F25" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
+      <c r="K25" s="10"/>
       <c r="L25" s="8"/>
       <c r="M25" s="26"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="24"/>
-      <c r="T25" s="24"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="26"/>
+      <c r="P25" s="26"/>
+      <c r="Q25" s="26"/>
+      <c r="R25" s="26"/>
+      <c r="S25" s="26"/>
+      <c r="T25" s="26"/>
       <c r="U25" s="8"/>
     </row>
     <row r="26" spans="2:21" ht="13.5" customHeight="1">
       <c r="B26" s="64">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26" s="69"/>
       <c r="D26" s="40"/>
       <c r="E26" s="68"/>
       <c r="F26" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
@@ -11244,7 +11747,7 @@
       <c r="D27" s="46"/>
       <c r="E27" s="46"/>
       <c r="F27" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
@@ -11264,13 +11767,13 @@
     </row>
     <row r="28" spans="2:21" ht="13.5" customHeight="1">
       <c r="B28" s="64">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C28" s="69"/>
       <c r="D28" s="40"/>
       <c r="E28" s="68"/>
       <c r="F28" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
@@ -11294,7 +11797,7 @@
       <c r="D29" s="46"/>
       <c r="E29" s="46"/>
       <c r="F29" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
@@ -11331,24 +11834,24 @@
     </row>
     <row r="31" spans="2:21" ht="15.75" customHeight="1">
       <c r="B31" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="2:21" ht="15.75" customHeight="1">
       <c r="B32" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="3:3" ht="15.75" customHeight="1"/>
     <row r="34" spans="3:3" ht="15.75" customHeight="1">
       <c r="C34" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="3:3" ht="15.75" customHeight="1"/>
@@ -12368,7 +12871,7 @@
   </sheetPr>
   <dimension ref="B1:E1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B29" sqref="B29:E47"/>
     </sheetView>
   </sheetViews>
@@ -12387,7 +12890,7 @@
     <row r="2" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="3" spans="2:5" ht="22.5" customHeight="1">
       <c r="B3" s="38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="39"/>
@@ -12408,7 +12911,7 @@
     <row r="6" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="7" spans="2:5" ht="30.75" customHeight="1">
       <c r="B7" s="74" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="47"/>
       <c r="D7" s="47"/>
@@ -12417,15 +12920,15 @@
     <row r="8" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="9" spans="2:5" ht="15.75" customHeight="1">
       <c r="B9" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" customHeight="1">
       <c r="B10" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="75">
         <v>45667</v>
@@ -12435,20 +12938,20 @@
     </row>
     <row r="11" spans="2:5" ht="15.75" customHeight="1">
       <c r="B11" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="76" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D11" s="47"/>
       <c r="E11" s="48"/>
     </row>
     <row r="12" spans="2:5" ht="50.25" customHeight="1">
       <c r="B12" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="47"/>
       <c r="E12" s="48"/>
@@ -12456,7 +12959,7 @@
     <row r="13" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="14" spans="2:5" ht="15.75" customHeight="1">
       <c r="B14" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="47"/>
       <c r="D14" s="47"/>
@@ -12464,7 +12967,7 @@
     </row>
     <row r="15" spans="2:5" ht="15.75" customHeight="1">
       <c r="B15" s="78" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
@@ -12502,7 +13005,7 @@
     </row>
     <row r="21" spans="2:5" ht="15.75" customHeight="1">
       <c r="B21" s="77" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="47"/>
       <c r="D21" s="47"/>
@@ -12510,7 +13013,7 @@
     </row>
     <row r="22" spans="2:5" ht="15.75" customHeight="1">
       <c r="B22" s="78" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C22" s="39"/>
       <c r="D22" s="39"/>
@@ -12548,7 +13051,7 @@
     </row>
     <row r="28" spans="2:5" ht="15.75" customHeight="1">
       <c r="B28" s="77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="47"/>
@@ -12670,7 +13173,7 @@
     </row>
     <row r="48" spans="2:5" ht="15.75" customHeight="1">
       <c r="B48" s="77" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" s="47"/>
       <c r="D48" s="47"/>
@@ -12678,7 +13181,7 @@
     </row>
     <row r="49" spans="2:5" ht="15.75" customHeight="1">
       <c r="B49" s="73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49" s="39"/>
       <c r="D49" s="39"/>
@@ -13694,7 +14197,7 @@
   </sheetPr>
   <dimension ref="B1:E1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A38" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A14" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -13735,7 +14238,7 @@
     <row r="6" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="7" spans="2:5" ht="30.75" customHeight="1">
       <c r="B7" s="74" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="47"/>
       <c r="D7" s="47"/>
@@ -13744,15 +14247,15 @@
     <row r="8" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="9" spans="2:5" ht="15.75" customHeight="1">
       <c r="B9" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" customHeight="1">
       <c r="B10" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="75">
         <v>45671</v>
@@ -13762,20 +14265,20 @@
     </row>
     <row r="11" spans="2:5" ht="15.75" customHeight="1">
       <c r="B11" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="76" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="47"/>
       <c r="E11" s="48"/>
     </row>
     <row r="12" spans="2:5" ht="50.25" customHeight="1">
       <c r="B12" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="76" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D12" s="47"/>
       <c r="E12" s="48"/>
@@ -13783,7 +14286,7 @@
     <row r="13" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="14" spans="2:5" ht="15.75" customHeight="1">
       <c r="B14" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="47"/>
       <c r="D14" s="47"/>
@@ -13791,7 +14294,7 @@
     </row>
     <row r="15" spans="2:5" ht="15.75" customHeight="1">
       <c r="B15" s="78" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
@@ -13829,7 +14332,7 @@
     </row>
     <row r="21" spans="2:5" ht="15.75" customHeight="1">
       <c r="B21" s="77" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="47"/>
       <c r="D21" s="47"/>
@@ -13837,7 +14340,7 @@
     </row>
     <row r="22" spans="2:5" ht="15.75" customHeight="1">
       <c r="B22" s="78" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C22" s="39"/>
       <c r="D22" s="39"/>
@@ -13875,7 +14378,7 @@
     </row>
     <row r="28" spans="2:5" ht="15.75" customHeight="1">
       <c r="B28" s="77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="47"/>
@@ -13997,7 +14500,7 @@
     </row>
     <row r="48" spans="2:5" ht="15.75" customHeight="1">
       <c r="B48" s="77" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" s="47"/>
       <c r="D48" s="47"/>
@@ -14005,7 +14508,7 @@
     </row>
     <row r="49" spans="2:5" ht="15.75" customHeight="1">
       <c r="B49" s="73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49" s="39"/>
       <c r="D49" s="39"/>
@@ -15021,8 +15524,8 @@
   </sheetPr>
   <dimension ref="B1:E1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:E20"/>
+    <sheetView showGridLines="0" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -15062,7 +15565,7 @@
     <row r="6" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="7" spans="2:5" ht="30.75" customHeight="1">
       <c r="B7" s="74" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="47"/>
       <c r="D7" s="47"/>
@@ -15071,38 +15574,38 @@
     <row r="8" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="9" spans="2:5" ht="15.75" customHeight="1">
       <c r="B9" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" customHeight="1">
       <c r="B10" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="75">
-        <v>45667</v>
+        <v>45678</v>
       </c>
       <c r="D10" s="47"/>
       <c r="E10" s="48"/>
     </row>
     <row r="11" spans="2:5" ht="15.75" customHeight="1">
       <c r="B11" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="76" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="47"/>
       <c r="E11" s="48"/>
     </row>
     <row r="12" spans="2:5" ht="50.25" customHeight="1">
       <c r="B12" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="47"/>
       <c r="E12" s="48"/>
@@ -15110,14 +15613,16 @@
     <row r="13" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="14" spans="2:5" ht="15.75" customHeight="1">
       <c r="B14" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="47"/>
       <c r="D14" s="47"/>
       <c r="E14" s="48"/>
     </row>
     <row r="15" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B15" s="78"/>
+      <c r="B15" s="78" t="s">
+        <v>81</v>
+      </c>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
       <c r="E15" s="40"/>
@@ -15154,7 +15659,7 @@
     </row>
     <row r="21" spans="2:5" ht="15.75" customHeight="1">
       <c r="B21" s="77" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="47"/>
       <c r="D21" s="47"/>
@@ -15162,7 +15667,7 @@
     </row>
     <row r="22" spans="2:5" ht="15.75" customHeight="1">
       <c r="B22" s="78" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="C22" s="39"/>
       <c r="D22" s="39"/>
@@ -15200,7 +15705,7 @@
     </row>
     <row r="28" spans="2:5" ht="15.75" customHeight="1">
       <c r="B28" s="77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="47"/>
@@ -15322,7 +15827,7 @@
     </row>
     <row r="48" spans="2:5" ht="15.75" customHeight="1">
       <c r="B48" s="77" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" s="47"/>
       <c r="D48" s="47"/>
@@ -15330,7 +15835,7 @@
     </row>
     <row r="49" spans="2:5" ht="15.75" customHeight="1">
       <c r="B49" s="73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49" s="39"/>
       <c r="D49" s="39"/>
@@ -16335,6 +16840,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -16345,8 +16851,8 @@
   </sheetPr>
   <dimension ref="B1:E1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -16386,7 +16892,7 @@
     <row r="6" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="7" spans="2:5" ht="30.75" customHeight="1">
       <c r="B7" s="74" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="47"/>
       <c r="D7" s="47"/>
@@ -16395,38 +16901,38 @@
     <row r="8" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="9" spans="2:5" ht="15.75" customHeight="1">
       <c r="B9" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" customHeight="1">
       <c r="B10" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="75">
-        <v>45667</v>
+        <v>45686</v>
       </c>
       <c r="D10" s="47"/>
       <c r="E10" s="48"/>
     </row>
     <row r="11" spans="2:5" ht="15.75" customHeight="1">
       <c r="B11" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="76" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="47"/>
       <c r="E11" s="48"/>
     </row>
     <row r="12" spans="2:5" ht="50.25" customHeight="1">
       <c r="B12" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="47"/>
       <c r="E12" s="48"/>
@@ -16434,14 +16940,16 @@
     <row r="13" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="14" spans="2:5" ht="15.75" customHeight="1">
       <c r="B14" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="47"/>
       <c r="D14" s="47"/>
       <c r="E14" s="48"/>
     </row>
     <row r="15" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B15" s="78"/>
+      <c r="B15" s="78" t="s">
+        <v>91</v>
+      </c>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
       <c r="E15" s="40"/>
@@ -16478,7 +16986,7 @@
     </row>
     <row r="21" spans="2:5" ht="15.75" customHeight="1">
       <c r="B21" s="77" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="47"/>
       <c r="D21" s="47"/>
@@ -16486,7 +16994,7 @@
     </row>
     <row r="22" spans="2:5" ht="15.75" customHeight="1">
       <c r="B22" s="78" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="C22" s="39"/>
       <c r="D22" s="39"/>
@@ -16524,7 +17032,7 @@
     </row>
     <row r="28" spans="2:5" ht="15.75" customHeight="1">
       <c r="B28" s="77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="47"/>
@@ -16646,7 +17154,7 @@
     </row>
     <row r="48" spans="2:5" ht="15.75" customHeight="1">
       <c r="B48" s="77" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" s="47"/>
       <c r="D48" s="47"/>
@@ -16654,7 +17162,7 @@
     </row>
     <row r="49" spans="2:5" ht="15.75" customHeight="1">
       <c r="B49" s="73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49" s="39"/>
       <c r="D49" s="39"/>
@@ -17659,6 +18167,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -17669,8 +18178,8 @@
   </sheetPr>
   <dimension ref="B1:E1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView showGridLines="0" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -17710,7 +18219,7 @@
     <row r="6" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="7" spans="2:5" ht="30.75" customHeight="1">
       <c r="B7" s="74" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="47"/>
       <c r="D7" s="47"/>
@@ -17719,38 +18228,38 @@
     <row r="8" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="9" spans="2:5" ht="15.75" customHeight="1">
       <c r="B9" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" customHeight="1">
       <c r="B10" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="75">
-        <v>45667</v>
+        <v>45663</v>
       </c>
       <c r="D10" s="47"/>
       <c r="E10" s="48"/>
     </row>
     <row r="11" spans="2:5" ht="15.75" customHeight="1">
       <c r="B11" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="76" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="47"/>
       <c r="E11" s="48"/>
     </row>
     <row r="12" spans="2:5" ht="50.25" customHeight="1">
       <c r="B12" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="47"/>
       <c r="E12" s="48"/>
@@ -17758,14 +18267,16 @@
     <row r="13" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="14" spans="2:5" ht="15.75" customHeight="1">
       <c r="B14" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="47"/>
       <c r="D14" s="47"/>
       <c r="E14" s="48"/>
     </row>
     <row r="15" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B15" s="78"/>
+      <c r="B15" s="78" t="s">
+        <v>89</v>
+      </c>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
       <c r="E15" s="40"/>
@@ -17802,7 +18313,7 @@
     </row>
     <row r="21" spans="2:5" ht="15.75" customHeight="1">
       <c r="B21" s="77" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="47"/>
       <c r="D21" s="47"/>
@@ -17810,7 +18321,7 @@
     </row>
     <row r="22" spans="2:5" ht="15.75" customHeight="1">
       <c r="B22" s="78" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="C22" s="39"/>
       <c r="D22" s="39"/>
@@ -17848,7 +18359,7 @@
     </row>
     <row r="28" spans="2:5" ht="15.75" customHeight="1">
       <c r="B28" s="77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="47"/>
@@ -17970,7 +18481,7 @@
     </row>
     <row r="48" spans="2:5" ht="15.75" customHeight="1">
       <c r="B48" s="77" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" s="47"/>
       <c r="D48" s="47"/>
@@ -17978,7 +18489,7 @@
     </row>
     <row r="49" spans="2:5" ht="15.75" customHeight="1">
       <c r="B49" s="73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49" s="39"/>
       <c r="D49" s="39"/>
@@ -18983,6 +19494,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -18993,8 +19505,8 @@
   </sheetPr>
   <dimension ref="B1:E1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -19034,7 +19546,7 @@
     <row r="6" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="7" spans="2:5" ht="30.75" customHeight="1">
       <c r="B7" s="74" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="47"/>
       <c r="D7" s="47"/>
@@ -19043,15 +19555,15 @@
     <row r="8" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="9" spans="2:5" ht="15.75" customHeight="1">
       <c r="B9" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" customHeight="1">
       <c r="B10" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="75">
         <v>45667</v>
@@ -19061,20 +19573,20 @@
     </row>
     <row r="11" spans="2:5" ht="15.75" customHeight="1">
       <c r="B11" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="76" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="47"/>
       <c r="E11" s="48"/>
     </row>
     <row r="12" spans="2:5" ht="50.25" customHeight="1">
       <c r="B12" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="47"/>
       <c r="E12" s="48"/>
@@ -19082,7 +19594,7 @@
     <row r="13" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="14" spans="2:5" ht="15.75" customHeight="1">
       <c r="B14" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="47"/>
       <c r="D14" s="47"/>
@@ -19126,7 +19638,7 @@
     </row>
     <row r="21" spans="2:5" ht="15.75" customHeight="1">
       <c r="B21" s="77" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="47"/>
       <c r="D21" s="47"/>
@@ -19134,7 +19646,7 @@
     </row>
     <row r="22" spans="2:5" ht="15.75" customHeight="1">
       <c r="B22" s="78" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" s="39"/>
       <c r="D22" s="39"/>
@@ -19172,7 +19684,7 @@
     </row>
     <row r="28" spans="2:5" ht="15.75" customHeight="1">
       <c r="B28" s="77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="47"/>
@@ -19294,7 +19806,7 @@
     </row>
     <row r="48" spans="2:5" ht="15.75" customHeight="1">
       <c r="B48" s="77" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" s="47"/>
       <c r="D48" s="47"/>
@@ -19302,7 +19814,7 @@
     </row>
     <row r="49" spans="2:5" ht="15.75" customHeight="1">
       <c r="B49" s="73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49" s="39"/>
       <c r="D49" s="39"/>
@@ -20358,7 +20870,7 @@
     <row r="6" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="7" spans="2:5" ht="30.75" customHeight="1">
       <c r="B7" s="74" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="47"/>
       <c r="D7" s="47"/>
@@ -20367,15 +20879,15 @@
     <row r="8" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="9" spans="2:5" ht="15.75" customHeight="1">
       <c r="B9" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" customHeight="1">
       <c r="B10" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="75">
         <v>45667</v>
@@ -20385,20 +20897,20 @@
     </row>
     <row r="11" spans="2:5" ht="15.75" customHeight="1">
       <c r="B11" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="76" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="47"/>
       <c r="E11" s="48"/>
     </row>
     <row r="12" spans="2:5" ht="50.25" customHeight="1">
       <c r="B12" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="47"/>
       <c r="E12" s="48"/>
@@ -20406,7 +20918,7 @@
     <row r="13" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="14" spans="2:5" ht="15.75" customHeight="1">
       <c r="B14" s="77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="47"/>
       <c r="D14" s="47"/>
@@ -20450,7 +20962,7 @@
     </row>
     <row r="21" spans="2:5" ht="15.75" customHeight="1">
       <c r="B21" s="77" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="47"/>
       <c r="D21" s="47"/>
@@ -20458,7 +20970,7 @@
     </row>
     <row r="22" spans="2:5" ht="15.75" customHeight="1">
       <c r="B22" s="78" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" s="39"/>
       <c r="D22" s="39"/>
@@ -20496,7 +21008,7 @@
     </row>
     <row r="28" spans="2:5" ht="15.75" customHeight="1">
       <c r="B28" s="77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="47"/>
@@ -20618,7 +21130,7 @@
     </row>
     <row r="48" spans="2:5" ht="15.75" customHeight="1">
       <c r="B48" s="77" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" s="47"/>
       <c r="D48" s="47"/>
@@ -20626,7 +21138,7 @@
     </row>
     <row r="49" spans="2:5" ht="15.75" customHeight="1">
       <c r="B49" s="73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49" s="39"/>
       <c r="D49" s="39"/>

</xml_diff>